<commit_message>
update SummaryBook before checking Friday group
</commit_message>
<xml_diff>
--- a/J00-Resources/SummaryBook.xlsx
+++ b/J00-Resources/SummaryBook.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>Andriy Zhidko - azhidko</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Java Courses Students list.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -544,7 +549,7 @@
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C3" t="s">
@@ -597,7 +602,13 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -605,23 +616,41 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
       <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -629,7 +658,13 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B8" s="2">
+        <v>8</v>
+      </c>
       <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -637,7 +672,13 @@
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
       <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -645,7 +686,13 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
       <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -653,7 +700,13 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
       <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -661,7 +714,13 @@
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
       <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -669,7 +728,13 @@
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
       <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -677,7 +742,13 @@
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
       <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -685,7 +756,11 @@
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -693,19 +768,30 @@
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
@@ -714,6 +800,7 @@
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
@@ -723,7 +810,8 @@
         <v>27</v>
       </c>
       <c r="B21" s="2">
-        <v>15</v>
+        <f>5+8</f>
+        <v>13</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -733,6 +821,7 @@
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
@@ -741,6 +830,7 @@
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
@@ -749,6 +839,9 @@
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B24" s="2">
+        <v>8</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
@@ -757,6 +850,7 @@
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>19</v>
       </c>
@@ -765,6 +859,7 @@
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
@@ -773,6 +868,9 @@
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>19</v>
       </c>
@@ -781,6 +879,7 @@
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>20</v>
       </c>
@@ -789,6 +888,7 @@
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
@@ -797,6 +897,7 @@
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>